<commit_message>
Insert sort impl (#1)
* using insert sort

* added some comments

---------

Co-authored-by: Alexey Seleznev <rib@live.ru>
</commit_message>
<xml_diff>
--- a/files/in.xlsx
+++ b/files/in.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rib\IdeaProjects\UdobSoftTask\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F14BFCB-F0AF-4539-B582-610E90E9BDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DE71A4-F582-4A33-AE1B-6F67A0D6488B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9531FC5F-CA38-4776-87D5-B4ABE163F13D}"/>
   </bookViews>
@@ -374,8 +374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB04D597-57B4-4525-8CC7-57FA241AF0DA}">
   <dimension ref="A1:A37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +522,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>